<commit_message>
changing color scale rule to make max and -max as the highest and lowest value
</commit_message>
<xml_diff>
--- a/components/data_analysis/median_color_map/quality_26_weeks.xlsx
+++ b/components/data_analysis/median_color_map/quality_26_weeks.xlsx
@@ -646,40 +646,40 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0017</v>
+        <v>-0.004</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.00215</v>
+        <v>-0.00153</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.00439</v>
+        <v>-0.00315</v>
       </c>
       <c r="E5" t="n">
-        <v>0.00233</v>
+        <v>-3.15e-05</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.000212</v>
+        <v>0.000621</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00392</v>
+        <v>0.0166</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.00177</v>
+        <v>-0.00132</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0008899999999999999</v>
+        <v>-0.000615</v>
       </c>
       <c r="J5" t="n">
-        <v>0.00173</v>
+        <v>0.000367</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.00242</v>
+        <v>-0.0016</v>
       </c>
       <c r="L5" t="n">
-        <v>0.00168</v>
+        <v>0.00228</v>
       </c>
       <c r="M5" t="n">
-        <v>0.00359</v>
+        <v>-0.001</v>
       </c>
     </row>
     <row r="6">
@@ -689,40 +689,40 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.00271</v>
+        <v>0.00244</v>
       </c>
       <c r="C6" t="n">
-        <v>0.00176</v>
+        <v>0.00121</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.00283</v>
+        <v>-5.87e-05</v>
       </c>
       <c r="E6" t="n">
-        <v>0.00197</v>
+        <v>-0.00205</v>
       </c>
       <c r="F6" t="n">
-        <v>0.008829999999999999</v>
+        <v>0.00551</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.00264</v>
+        <v>0.0155</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0009300000000000001</v>
+        <v>-0.00137</v>
       </c>
       <c r="I6" t="n">
-        <v>0.000521</v>
+        <v>-0.000614</v>
       </c>
       <c r="J6" t="n">
-        <v>0.00117</v>
+        <v>0.00129</v>
       </c>
       <c r="K6" t="n">
-        <v>0.00051</v>
+        <v>-1.55e-05</v>
       </c>
       <c r="L6" t="n">
-        <v>0.00357</v>
+        <v>0.0024</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0074</v>
+        <v>0.0015</v>
       </c>
     </row>
     <row r="7">
@@ -732,40 +732,40 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.00369</v>
+        <v>0.00109</v>
       </c>
       <c r="C7" t="n">
-        <v>0.00053</v>
+        <v>-0.00372</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0049</v>
+        <v>0.00791</v>
       </c>
       <c r="E7" t="n">
-        <v>0.00225</v>
+        <v>0.00164</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.000635</v>
+        <v>0.000428</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.007860000000000001</v>
+        <v>0.00788</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.000925</v>
+        <v>-0.00188</v>
       </c>
       <c r="I7" t="n">
-        <v>0.00256</v>
+        <v>0.00121</v>
       </c>
       <c r="J7" t="n">
-        <v>0.00478</v>
+        <v>0.00516</v>
       </c>
       <c r="K7" t="n">
-        <v>0.00302</v>
+        <v>0.00193</v>
       </c>
       <c r="L7" t="n">
-        <v>0.00198</v>
+        <v>0.00153</v>
       </c>
       <c r="M7" t="n">
-        <v>0.00223</v>
+        <v>0.00627</v>
       </c>
     </row>
     <row r="8">
@@ -775,40 +775,40 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.00128</v>
+        <v>-0.00234</v>
       </c>
       <c r="C8" t="n">
-        <v>0.00108</v>
+        <v>-0.000597</v>
       </c>
       <c r="D8" t="n">
-        <v>0.00411</v>
+        <v>-0.00358</v>
       </c>
       <c r="E8" t="n">
-        <v>0.00783</v>
+        <v>0.00732</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.00359</v>
+        <v>-0.0019</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.00332</v>
+        <v>0.0108</v>
       </c>
       <c r="H8" t="n">
-        <v>0.00247</v>
+        <v>-0.00242</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.0005509999999999999</v>
+        <v>-0.000452</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.00547</v>
+        <v>-0.00315</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.00284</v>
+        <v>0.000469</v>
       </c>
       <c r="L8" t="n">
-        <v>0.00171</v>
+        <v>0.00245</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.0031</v>
+        <v>-0.000226</v>
       </c>
     </row>
     <row r="9">
@@ -818,40 +818,40 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0201</v>
+        <v>0.0166</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.0027</v>
+        <v>-0.00236</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.000349</v>
+        <v>-0.00492</v>
       </c>
       <c r="E9" t="n">
-        <v>0.000678</v>
+        <v>0.00419</v>
       </c>
       <c r="F9" t="n">
-        <v>0.000891</v>
+        <v>0.000992</v>
       </c>
       <c r="G9" t="n">
-        <v>0.00347</v>
+        <v>0.00486</v>
       </c>
       <c r="H9" t="n">
-        <v>9.19e-05</v>
+        <v>0.000589</v>
       </c>
       <c r="I9" t="n">
-        <v>8.780000000000001e-05</v>
+        <v>0.000105</v>
       </c>
       <c r="J9" t="n">
-        <v>0.00165</v>
+        <v>0.00137</v>
       </c>
       <c r="K9" t="n">
-        <v>0.00177</v>
+        <v>0.00249</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.00049</v>
+        <v>0.000148</v>
       </c>
       <c r="M9" t="n">
-        <v>0.000212</v>
+        <v>0.0027</v>
       </c>
     </row>
     <row r="10">
@@ -861,40 +861,40 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0195</v>
+        <v>0.00578</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0193</v>
+        <v>0.00331</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0109</v>
+        <v>0.00269</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0251</v>
+        <v>0.00518</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0226</v>
+        <v>0.00257</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0163</v>
+        <v>-0.00895</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0114</v>
+        <v>0.00735</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0135</v>
+        <v>0.00597</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0171</v>
+        <v>0.008370000000000001</v>
       </c>
       <c r="K10" t="n">
-        <v>0.00893</v>
+        <v>0.00427</v>
       </c>
       <c r="L10" t="n">
-        <v>0.0164</v>
+        <v>0.00424</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0117</v>
+        <v>0.00627</v>
       </c>
     </row>
     <row r="11">
@@ -904,40 +904,40 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.00217</v>
+        <v>-0.00305</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.00516</v>
+        <v>0.00146</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.00339</v>
+        <v>-0.00219</v>
       </c>
       <c r="E11" t="n">
-        <v>0.000157</v>
+        <v>0.000309</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.00373</v>
+        <v>-0.0049</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.00293</v>
+        <v>-0.00127</v>
       </c>
       <c r="H11" t="n">
-        <v>0.00144</v>
+        <v>0.00036</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.00251</v>
+        <v>-0.00126</v>
       </c>
       <c r="J11" t="n">
-        <v>0.00159</v>
+        <v>-5.85e-05</v>
       </c>
       <c r="K11" t="n">
-        <v>-7.949999999999999e-05</v>
+        <v>0.0017</v>
       </c>
       <c r="L11" t="n">
-        <v>0.00111</v>
+        <v>-0.000662</v>
       </c>
       <c r="M11" t="n">
-        <v>-0.00183</v>
+        <v>-0.00127</v>
       </c>
     </row>
     <row r="12">
@@ -947,40 +947,40 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.00216</v>
+        <v>-0.00485</v>
       </c>
       <c r="C12" t="n">
-        <v>-2.36e-05</v>
+        <v>2.29e-05</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.00332</v>
+        <v>0.00171</v>
       </c>
       <c r="E12" t="n">
-        <v>0.00187</v>
+        <v>-0.000326</v>
       </c>
       <c r="F12" t="n">
-        <v>0.00695</v>
+        <v>0.00129</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.00135</v>
+        <v>0.008699999999999999</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.000168</v>
+        <v>-0.00127</v>
       </c>
       <c r="I12" t="n">
-        <v>0.00344</v>
+        <v>-0.000637</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.00279</v>
+        <v>-0.00224</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.007889999999999999</v>
+        <v>-0.00532</v>
       </c>
       <c r="L12" t="n">
-        <v>-0.000215</v>
+        <v>-0.00137</v>
       </c>
       <c r="M12" t="n">
-        <v>0.000831</v>
+        <v>-0.00252</v>
       </c>
     </row>
     <row r="13">
@@ -990,40 +990,40 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.00676</v>
+        <v>-0.0121</v>
       </c>
       <c r="C13" t="n">
-        <v>0.00202</v>
+        <v>-0.00204</v>
       </c>
       <c r="D13" t="n">
-        <v>0.00157</v>
+        <v>0.00232</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.000262</v>
+        <v>0.00056</v>
       </c>
       <c r="F13" t="n">
-        <v>0.00826</v>
+        <v>0.00564</v>
       </c>
       <c r="G13" t="n">
-        <v>0.00382</v>
+        <v>0.0113</v>
       </c>
       <c r="H13" t="n">
-        <v>0.000585</v>
+        <v>-0.00014</v>
       </c>
       <c r="I13" t="n">
-        <v>0.00264</v>
+        <v>0.000964</v>
       </c>
       <c r="J13" t="n">
-        <v>0.00425</v>
+        <v>-0.000687</v>
       </c>
       <c r="K13" t="n">
-        <v>0.00166</v>
+        <v>-0.00283</v>
       </c>
       <c r="L13" t="n">
-        <v>0.008030000000000001</v>
+        <v>0.0038</v>
       </c>
       <c r="M13" t="n">
-        <v>0.00461</v>
+        <v>-0.00041</v>
       </c>
     </row>
     <row r="14">
@@ -1033,40 +1033,40 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.00015</v>
+        <v>0.000108</v>
       </c>
       <c r="C14" t="n">
-        <v>0.00138</v>
+        <v>-0.00373</v>
       </c>
       <c r="D14" t="n">
-        <v>0.00153</v>
+        <v>0.00455</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.00266</v>
+        <v>-0.00253</v>
       </c>
       <c r="F14" t="n">
-        <v>3.28e-05</v>
+        <v>-0.000736</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.00156</v>
+        <v>0.0114</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0015</v>
+        <v>-0.00139</v>
       </c>
       <c r="I14" t="n">
-        <v>0.00139</v>
+        <v>9.31e-05</v>
       </c>
       <c r="J14" t="n">
-        <v>0.000249</v>
+        <v>0.000934</v>
       </c>
       <c r="K14" t="n">
-        <v>0.00385</v>
+        <v>0.00143</v>
       </c>
       <c r="L14" t="n">
-        <v>0.00542</v>
+        <v>0.00348</v>
       </c>
       <c r="M14" t="n">
-        <v>0.00284</v>
+        <v>-0.000281</v>
       </c>
     </row>
   </sheetData>
@@ -1080,9 +1080,9 @@
   <conditionalFormatting sqref="B5:D14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="percentile" val="1"/>
         <cfvo type="num" val="0"/>
-        <cfvo type="max"/>
+        <cfvo type="percentile" val="-100"/>
         <color rgb="00FF0000"/>
         <color rgb="00FFFFFF"/>
         <color rgb="00228B22"/>
@@ -1090,11 +1090,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:G14">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="percentile" val="1"/>
         <cfvo type="num" val="0"/>
-        <cfvo type="max"/>
+        <cfvo type="percentile" val="-100"/>
         <color rgb="00FF0000"/>
         <color rgb="00FFFFFF"/>
         <color rgb="00228B22"/>
@@ -1102,11 +1102,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:J14">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="percentile" val="1"/>
         <cfvo type="num" val="0"/>
-        <cfvo type="max"/>
+        <cfvo type="percentile" val="-100"/>
         <color rgb="00FF0000"/>
         <color rgb="00FFFFFF"/>
         <color rgb="00228B22"/>
@@ -1114,11 +1114,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:M14">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="percentile" val="1"/>
         <cfvo type="num" val="0"/>
-        <cfvo type="max"/>
+        <cfvo type="percentile" val="-100"/>
         <color rgb="00FF0000"/>
         <color rgb="00FFFFFF"/>
         <color rgb="00228B22"/>

</xml_diff>